<commit_message>
move animation and excel
</commit_message>
<xml_diff>
--- a/src/Duelyst/Database/DuelystCards.xlsx
+++ b/src/Duelyst/Database/DuelystCards.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>ManaCost</t>
   </si>
@@ -57,9 +57,6 @@
     <t>SiavashDesc</t>
   </si>
   <si>
-    <t>HERO</t>
-  </si>
-  <si>
     <t>MELEE</t>
   </si>
   <si>
@@ -67,6 +64,39 @@
   </si>
   <si>
     <t>./res/Characters/generals/general_f1.png</t>
+  </si>
+  <si>
+    <t>Address of Idle Gif</t>
+  </si>
+  <si>
+    <t>./res/gifs/f1_altgeneral/idle_t.gif</t>
+  </si>
+  <si>
+    <t>MINION</t>
+  </si>
+  <si>
+    <t>Address of Run Gif</t>
+  </si>
+  <si>
+    <t>./res/gifs/f1_altgeneral/run_t.gif</t>
+  </si>
+  <si>
+    <t>Address of Attack Gif</t>
+  </si>
+  <si>
+    <t>./res/gifs/f1_altgeneral/attack_t.gif</t>
+  </si>
+  <si>
+    <t>Address of Get Damage Gif</t>
+  </si>
+  <si>
+    <t>FRIENDLY</t>
+  </si>
+  <si>
+    <t>Address Of Death Gif</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Target Society</t>
   </si>
 </sst>
 </file>
@@ -384,28 +414,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="24.7109375" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" customWidth="1"/>
-    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="2" max="2" width="36.5703125" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" customWidth="1"/>
+    <col min="4" max="4" width="25" customWidth="1"/>
+    <col min="5" max="5" width="23" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
     <col min="7" max="7" width="17.42578125" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
     <col min="9" max="9" width="12.5703125" customWidth="1"/>
     <col min="10" max="10" width="11.42578125" customWidth="1"/>
     <col min="11" max="11" width="49.42578125" customWidth="1"/>
+    <col min="12" max="12" width="34.42578125" customWidth="1"/>
+    <col min="13" max="13" width="39.7109375" customWidth="1"/>
+    <col min="14" max="14" width="36.140625" customWidth="1"/>
+    <col min="15" max="15" width="38.42578125" customWidth="1"/>
+    <col min="16" max="16" width="41.85546875" customWidth="1"/>
+    <col min="17" max="17" width="33.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -437,10 +473,28 @@
         <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="L1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -448,7 +502,7 @@
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -457,7 +511,7 @@
         <v>50</v>
       </c>
       <c r="F2">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="G2">
         <v>20</v>
@@ -466,13 +520,31 @@
         <v>2</v>
       </c>
       <c r="I2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J2">
         <v>0</v>
       </c>
       <c r="K2" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="L2" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
A Lot of Attack Elements Done
</commit_message>
<xml_diff>
--- a/src/Duelyst/Database/DuelystCards.xlsx
+++ b/src/Duelyst/Database/DuelystCards.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>ManaCost</t>
   </si>
@@ -97,6 +97,12 @@
   </si>
   <si>
     <t xml:space="preserve"> Target Society</t>
+  </si>
+  <si>
+    <t>./res/gifs/f1_altgeneral/hit_t.gif</t>
+  </si>
+  <si>
+    <t>./res/gifs/f1_altgeneral/death_t.gif</t>
   </si>
 </sst>
 </file>
@@ -416,8 +422,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="O27" sqref="O27"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,10 +544,10 @@
         <v>21</v>
       </c>
       <c r="O2" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="P2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="Q2" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
A Big Performance Fix
</commit_message>
<xml_diff>
--- a/src/Duelyst/Database/DuelystCards.xlsx
+++ b/src/Duelyst/Database/DuelystCards.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asus\Desktop\Duelyst_java8\src\Duelyst\Database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\_Downloads\Comperessed\Duelyst_java8\src\Duelyst\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14772" windowHeight="8160"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14775" windowHeight="8160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="113">
   <si>
     <t>ManaCost</t>
   </si>
@@ -358,15 +358,12 @@
   </si>
   <si>
     <t>Rostam</t>
-  </si>
-  <si>
-    <t>Null</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -680,32 +677,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="93" workbookViewId="0">
-      <selection activeCell="V18" sqref="V18"/>
+    <sheetView tabSelected="1" topLeftCell="L26" zoomScale="93" workbookViewId="0">
+      <selection activeCell="P54" sqref="P54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.109375" customWidth="1"/>
-    <col min="2" max="2" width="36.5546875" customWidth="1"/>
-    <col min="3" max="3" width="27.44140625" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="90.42578125" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
     <col min="5" max="5" width="23" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="7" max="7" width="17.44140625" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
-    <col min="9" max="9" width="12.5546875" customWidth="1"/>
-    <col min="10" max="10" width="11.44140625" customWidth="1"/>
-    <col min="11" max="11" width="49.44140625" customWidth="1"/>
-    <col min="12" max="12" width="34.44140625" customWidth="1"/>
-    <col min="13" max="13" width="39.6640625" customWidth="1"/>
-    <col min="14" max="14" width="36.109375" customWidth="1"/>
-    <col min="15" max="15" width="38.44140625" customWidth="1"/>
-    <col min="16" max="16" width="41.88671875" customWidth="1"/>
-    <col min="17" max="17" width="33.109375" customWidth="1"/>
+    <col min="9" max="9" width="12.5703125" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" customWidth="1"/>
+    <col min="11" max="11" width="49.42578125" customWidth="1"/>
+    <col min="12" max="12" width="34.42578125" customWidth="1"/>
+    <col min="13" max="13" width="39.7109375" customWidth="1"/>
+    <col min="14" max="14" width="36.140625" customWidth="1"/>
+    <col min="15" max="15" width="38.42578125" customWidth="1"/>
+    <col min="16" max="16" width="41.85546875" customWidth="1"/>
+    <col min="17" max="17" width="33.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -758,7 +755,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -811,7 +808,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -843,28 +840,28 @@
         <v>0</v>
       </c>
       <c r="K3" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="L3" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="M3" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="N3" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="O3" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="P3" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="Q3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -896,28 +893,28 @@
         <v>0</v>
       </c>
       <c r="K4" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="L4" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="M4" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="N4" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="O4" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="P4" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="Q4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -949,28 +946,28 @@
         <v>0</v>
       </c>
       <c r="K5" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="L5" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="M5" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="N5" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="O5" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="P5" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="Q5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -1002,28 +999,28 @@
         <v>0</v>
       </c>
       <c r="K6" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="L6" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="M6" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="N6" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="O6" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="P6" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="Q6" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -1055,28 +1052,28 @@
         <v>0</v>
       </c>
       <c r="K7" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="L7" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="M7" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="N7" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="O7" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="P7" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="Q7" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -1108,28 +1105,28 @@
         <v>0</v>
       </c>
       <c r="K8" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="L8" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="M8" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="N8" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="O8" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="P8" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="Q8" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -1161,28 +1158,28 @@
         <v>0</v>
       </c>
       <c r="K9" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="L9" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="M9" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="N9" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="O9" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="P9" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="Q9" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -1214,28 +1211,28 @@
         <v>0</v>
       </c>
       <c r="K10" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="L10" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="M10" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="N10" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="O10" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="P10" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="Q10" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -1267,28 +1264,28 @@
         <v>0</v>
       </c>
       <c r="K11" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="L11" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="M11" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="N11" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="O11" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="P11" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="Q11" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -1320,28 +1317,28 @@
         <v>0</v>
       </c>
       <c r="K12" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="L12" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="M12" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="N12" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="O12" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="P12" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="Q12" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>44</v>
       </c>
@@ -1373,28 +1370,28 @@
         <v>0</v>
       </c>
       <c r="K13" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="L13" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="M13" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="N13" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="O13" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="P13" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="Q13" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -1426,28 +1423,28 @@
         <v>0</v>
       </c>
       <c r="K14" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="L14" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="M14" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="N14" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="O14" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="P14" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="Q14" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -1479,28 +1476,28 @@
         <v>0</v>
       </c>
       <c r="K15" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="L15" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="M15" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="N15" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="O15" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="P15" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="Q15" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>47</v>
       </c>
@@ -1532,28 +1529,28 @@
         <v>0</v>
       </c>
       <c r="K16" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="L16" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="M16" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="N16" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="O16" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="P16" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="Q16" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -1585,28 +1582,28 @@
         <v>0</v>
       </c>
       <c r="K17" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="L17" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="M17" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="N17" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="O17" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="P17" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="Q17" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>50</v>
       </c>
@@ -1638,28 +1635,28 @@
         <v>0</v>
       </c>
       <c r="K18" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="L18" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="M18" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="N18" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="O18" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="P18" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="Q18" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>52</v>
       </c>
@@ -1691,28 +1688,28 @@
         <v>0</v>
       </c>
       <c r="K19" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="L19" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="M19" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="N19" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="O19" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="P19" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="Q19" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>54</v>
       </c>
@@ -1744,28 +1741,28 @@
         <v>0</v>
       </c>
       <c r="K20" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="L20" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="M20" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="N20" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="O20" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="P20" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="Q20" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>55</v>
       </c>
@@ -1797,28 +1794,28 @@
         <v>0</v>
       </c>
       <c r="K21" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="L21" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="M21" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="N21" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="O21" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="P21" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="Q21" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>57</v>
       </c>
@@ -1850,28 +1847,28 @@
         <v>0</v>
       </c>
       <c r="K22" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="L22" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="M22" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="N22" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="O22" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="P22" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="Q22" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>59</v>
       </c>
@@ -1903,28 +1900,28 @@
         <v>0</v>
       </c>
       <c r="K23" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="L23" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="M23" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="N23" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="O23" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="P23" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="Q23" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>61</v>
       </c>
@@ -1956,28 +1953,28 @@
         <v>0</v>
       </c>
       <c r="K24" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="L24" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="M24" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="N24" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="O24" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="P24" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="Q24" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>63</v>
       </c>
@@ -2009,28 +2006,28 @@
         <v>0</v>
       </c>
       <c r="K25" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="L25" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="M25" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="N25" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="O25" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="P25" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="Q25" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>65</v>
       </c>
@@ -2062,28 +2059,28 @@
         <v>0</v>
       </c>
       <c r="K26" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="L26" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="M26" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="N26" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="O26" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="P26" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="Q26" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>67</v>
       </c>
@@ -2115,28 +2112,28 @@
         <v>0</v>
       </c>
       <c r="K27" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="L27" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="M27" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="N27" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="O27" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="P27" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="Q27" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>69</v>
       </c>
@@ -2168,28 +2165,28 @@
         <v>0</v>
       </c>
       <c r="K28" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="L28" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="M28" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="N28" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="O28" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="P28" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="Q28" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>71</v>
       </c>
@@ -2221,28 +2218,28 @@
         <v>0</v>
       </c>
       <c r="K29" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="L29" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="M29" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="N29" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="O29" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="P29" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="Q29" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>73</v>
       </c>
@@ -2274,28 +2271,28 @@
         <v>0</v>
       </c>
       <c r="K30" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="L30" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="M30" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="N30" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="O30" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="P30" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="Q30" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>75</v>
       </c>
@@ -2327,28 +2324,28 @@
         <v>0</v>
       </c>
       <c r="K31" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="L31" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="M31" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="N31" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="O31" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="P31" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="Q31" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>77</v>
       </c>
@@ -2380,28 +2377,28 @@
         <v>0</v>
       </c>
       <c r="K32" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="L32" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="M32" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="N32" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="O32" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="P32" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="Q32" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>79</v>
       </c>
@@ -2433,28 +2430,28 @@
         <v>0</v>
       </c>
       <c r="K33" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="L33" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="M33" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="N33" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="O33" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="P33" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="Q33" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>81</v>
       </c>
@@ -2486,28 +2483,28 @@
         <v>0</v>
       </c>
       <c r="K34" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="L34" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="M34" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="N34" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="O34" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="P34" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="Q34" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>82</v>
       </c>
@@ -2539,28 +2536,28 @@
         <v>0</v>
       </c>
       <c r="K35" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="L35" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="M35" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="N35" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="O35" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="P35" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="Q35" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>83</v>
       </c>
@@ -2592,28 +2589,28 @@
         <v>0</v>
       </c>
       <c r="K36" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="L36" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="M36" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="N36" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="O36" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="P36" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="Q36" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>85</v>
       </c>
@@ -2645,28 +2642,28 @@
         <v>0</v>
       </c>
       <c r="K37" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="L37" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="M37" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="N37" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="O37" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="P37" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="Q37" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>87</v>
       </c>
@@ -2698,28 +2695,28 @@
         <v>0</v>
       </c>
       <c r="K38" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="L38" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="M38" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="N38" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="O38" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="P38" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="Q38" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>89</v>
       </c>
@@ -2751,28 +2748,28 @@
         <v>0</v>
       </c>
       <c r="K39" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="L39" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="M39" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="N39" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="O39" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="P39" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="Q39" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>91</v>
       </c>
@@ -2804,28 +2801,28 @@
         <v>0</v>
       </c>
       <c r="K40" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="L40" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="M40" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="N40" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="O40" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="P40" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="Q40" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>92</v>
       </c>
@@ -2857,28 +2854,28 @@
         <v>0</v>
       </c>
       <c r="K41" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="L41" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="M41" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="N41" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="O41" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="P41" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="Q41" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>93</v>
       </c>
@@ -2910,28 +2907,28 @@
         <v>0</v>
       </c>
       <c r="K42" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="L42" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="M42" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="N42" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="O42" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="P42" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="Q42" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>96</v>
       </c>
@@ -2963,28 +2960,28 @@
         <v>0</v>
       </c>
       <c r="K43" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="L43" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="M43" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="N43" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="O43" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="P43" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="Q43" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>98</v>
       </c>
@@ -3016,28 +3013,28 @@
         <v>0</v>
       </c>
       <c r="K44" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="L44" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="M44" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="N44" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="O44" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="P44" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="Q44" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>100</v>
       </c>
@@ -3069,28 +3066,28 @@
         <v>0</v>
       </c>
       <c r="K45" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="L45" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="M45" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="N45" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="O45" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="P45" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="Q45" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>102</v>
       </c>
@@ -3122,28 +3119,28 @@
         <v>0</v>
       </c>
       <c r="K46" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="L46" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="M46" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="N46" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="O46" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="P46" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="Q46" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>104</v>
       </c>
@@ -3175,28 +3172,28 @@
         <v>0</v>
       </c>
       <c r="K47" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="L47" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="M47" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="N47" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="O47" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="P47" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="Q47" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>106</v>
       </c>
@@ -3228,28 +3225,28 @@
         <v>0</v>
       </c>
       <c r="K48" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="L48" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="M48" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="N48" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="O48" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="P48" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="Q48" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>108</v>
       </c>
@@ -3281,28 +3278,28 @@
         <v>0</v>
       </c>
       <c r="K49" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="L49" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="M49" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="N49" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="O49" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="P49" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="Q49" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>110</v>
       </c>
@@ -3334,28 +3331,28 @@
         <v>0</v>
       </c>
       <c r="K50" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="L50" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="M50" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="N50" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="O50" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="P50" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="Q50" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>112</v>
       </c>
@@ -3387,25 +3384,25 @@
         <v>0</v>
       </c>
       <c r="K51" t="s">
-        <v>113</v>
+        <v>12</v>
       </c>
       <c r="L51" t="s">
-        <v>113</v>
+        <v>14</v>
       </c>
       <c r="M51" t="s">
-        <v>113</v>
+        <v>17</v>
       </c>
       <c r="N51" t="s">
-        <v>113</v>
+        <v>19</v>
       </c>
       <c r="O51" t="s">
-        <v>113</v>
+        <v>24</v>
       </c>
       <c r="P51" t="s">
-        <v>113</v>
+        <v>25</v>
       </c>
       <c r="Q51" t="s">
-        <v>113</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Card Creator Some things done.
</commit_message>
<xml_diff>
--- a/src/Duelyst/Database/DuelystCards.xlsx
+++ b/src/Duelyst/Database/DuelystCards.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="567" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="114">
   <si>
     <t>ManaCost</t>
   </si>
@@ -358,6 +358,9 @@
   </si>
   <si>
     <t>Rostam</t>
+  </si>
+  <si>
+    <t>Cooldown</t>
   </si>
 </sst>
 </file>
@@ -675,15 +678,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q51"/>
+  <dimension ref="A1:R51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L26" zoomScale="93" workbookViewId="0">
-      <selection activeCell="P54" sqref="P54"/>
+    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection activeCell="A5" sqref="A5"/>
+      <selection pane="topRight" activeCell="Z41" sqref="Z41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="1" max="1" width="22.28515625" customWidth="1"/>
     <col min="2" max="2" width="90.42578125" customWidth="1"/>
     <col min="3" max="3" width="27.42578125" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
@@ -702,7 +707,7 @@
     <col min="17" max="17" width="33.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -754,8 +759,11 @@
       <c r="Q1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>26</v>
       </c>
@@ -807,8 +815,11 @@
       <c r="Q2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -860,8 +871,11 @@
       <c r="Q3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -913,8 +927,11 @@
       <c r="Q4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>33</v>
       </c>
@@ -966,8 +983,11 @@
       <c r="Q5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>34</v>
       </c>
@@ -1019,8 +1039,11 @@
       <c r="Q6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -1072,8 +1095,11 @@
       <c r="Q7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -1125,8 +1151,11 @@
       <c r="Q8" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -1178,8 +1207,11 @@
       <c r="Q9" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -1231,8 +1263,11 @@
       <c r="Q10" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -1284,8 +1319,11 @@
       <c r="Q11" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -1337,8 +1375,11 @@
       <c r="Q12" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>44</v>
       </c>
@@ -1390,8 +1431,11 @@
       <c r="Q13" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -1443,8 +1487,11 @@
       <c r="Q14" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -1496,8 +1543,11 @@
       <c r="Q15" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>47</v>
       </c>
@@ -1549,8 +1599,11 @@
       <c r="Q16" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -1602,8 +1655,11 @@
       <c r="Q17" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>50</v>
       </c>
@@ -1655,8 +1711,11 @@
       <c r="Q18" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>52</v>
       </c>
@@ -1708,8 +1767,11 @@
       <c r="Q19" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>54</v>
       </c>
@@ -1761,8 +1823,11 @@
       <c r="Q20" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>55</v>
       </c>
@@ -1814,8 +1879,11 @@
       <c r="Q21" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>57</v>
       </c>
@@ -1867,8 +1935,11 @@
       <c r="Q22" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>59</v>
       </c>
@@ -1920,8 +1991,11 @@
       <c r="Q23" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>61</v>
       </c>
@@ -1973,8 +2047,11 @@
       <c r="Q24" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>63</v>
       </c>
@@ -2026,8 +2103,11 @@
       <c r="Q25" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>65</v>
       </c>
@@ -2079,8 +2159,11 @@
       <c r="Q26" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>67</v>
       </c>
@@ -2132,8 +2215,11 @@
       <c r="Q27" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>69</v>
       </c>
@@ -2185,8 +2271,11 @@
       <c r="Q28" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>71</v>
       </c>
@@ -2238,8 +2327,11 @@
       <c r="Q29" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>73</v>
       </c>
@@ -2291,8 +2383,11 @@
       <c r="Q30" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>75</v>
       </c>
@@ -2344,8 +2439,11 @@
       <c r="Q31" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>77</v>
       </c>
@@ -2397,8 +2495,11 @@
       <c r="Q32" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>79</v>
       </c>
@@ -2450,8 +2551,11 @@
       <c r="Q33" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>81</v>
       </c>
@@ -2503,8 +2607,11 @@
       <c r="Q34" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>82</v>
       </c>
@@ -2556,8 +2663,11 @@
       <c r="Q35" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>83</v>
       </c>
@@ -2609,8 +2719,11 @@
       <c r="Q36" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>85</v>
       </c>
@@ -2662,8 +2775,11 @@
       <c r="Q37" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>87</v>
       </c>
@@ -2715,8 +2831,11 @@
       <c r="Q38" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>89</v>
       </c>
@@ -2768,8 +2887,11 @@
       <c r="Q39" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>91</v>
       </c>
@@ -2821,8 +2943,11 @@
       <c r="Q40" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>92</v>
       </c>
@@ -2874,8 +2999,11 @@
       <c r="Q41" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>93</v>
       </c>
@@ -2927,8 +3055,11 @@
       <c r="Q42" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>96</v>
       </c>
@@ -2980,8 +3111,11 @@
       <c r="Q43" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R43">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>98</v>
       </c>
@@ -3033,8 +3167,11 @@
       <c r="Q44" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>100</v>
       </c>
@@ -3086,8 +3223,11 @@
       <c r="Q45" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>102</v>
       </c>
@@ -3139,8 +3279,11 @@
       <c r="Q46" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>104</v>
       </c>
@@ -3192,8 +3335,11 @@
       <c r="Q47" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>106</v>
       </c>
@@ -3245,8 +3391,11 @@
       <c r="Q48" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R48">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>108</v>
       </c>
@@ -3298,8 +3447,11 @@
       <c r="Q49" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>110</v>
       </c>
@@ -3351,8 +3503,11 @@
       <c r="Q50" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="R50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>112</v>
       </c>
@@ -3403,6 +3558,9 @@
       </c>
       <c r="Q51" t="s">
         <v>21</v>
+      </c>
+      <c r="R51">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Card creator image and add to shop and collection done
</commit_message>
<xml_diff>
--- a/src/Duelyst/Database/DuelystCards.xlsx
+++ b/src/Duelyst/Database/DuelystCards.xlsx
@@ -680,10 +680,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="93" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="L1" activePane="topRight" state="frozen"/>
       <selection activeCell="A5" sqref="A5"/>
-      <selection pane="topRight" activeCell="Z41" sqref="Z41"/>
+      <selection pane="topRight" activeCell="Q53" sqref="Q53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>